<commit_message>
updated activity till excel form
</commit_message>
<xml_diff>
--- a/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
+++ b/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
@@ -375,7 +375,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -408,13 +408,13 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C2" t="str">
-        <v>30</v>
+        <v>2</v>
       </c>
       <c r="D2" t="str">
-        <v>30</v>
+        <v>3</v>
       </c>
       <c r="E2" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="F2" t="str">
         <v>0</v>
@@ -428,16 +428,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C3" t="str">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D3" t="str">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E3" t="str">
+        <v>5</v>
+      </c>
+      <c r="F3" t="str">
         <v>1</v>
-      </c>
-      <c r="F3" t="str">
-        <v>4</v>
       </c>
     </row>
     <row r="4">
@@ -448,13 +448,13 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C4" t="str">
+        <v>30</v>
+      </c>
+      <c r="D4" t="str">
+        <v>30</v>
+      </c>
+      <c r="E4" t="str">
         <v>2</v>
-      </c>
-      <c r="D4" t="str">
-        <v>3</v>
-      </c>
-      <c r="E4" t="str">
-        <v>0</v>
       </c>
       <c r="F4" t="str">
         <v>0</v>
@@ -468,16 +468,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C5" t="str">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="D5" t="str">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="E5" t="str">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="F5" t="str">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="6">
@@ -488,16 +488,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C6" t="str">
-        <v>41</v>
+        <v>30</v>
       </c>
       <c r="D6" t="str">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="E6" t="str">
         <v>3</v>
       </c>
       <c r="F6" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7">
@@ -508,16 +508,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C7" t="str">
-        <v>39</v>
+        <v>13</v>
       </c>
       <c r="D7" t="str">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="E7" t="str">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="F7" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -528,16 +528,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C8" t="str">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D8" t="str">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="E8" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F8" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -548,16 +548,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C9" t="str">
-        <v>8</v>
+        <v>45</v>
       </c>
       <c r="D9" t="str">
-        <v>9</v>
+        <v>25</v>
       </c>
       <c r="E9" t="str">
         <v>1</v>
       </c>
       <c r="F9" t="str">
-        <v>0</v>
+        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -568,13 +568,13 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C10" t="str">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D10" t="str">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E10" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F10" t="str">
         <v>0</v>
@@ -600,9 +600,29 @@
         <v>3</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="str">
+        <v xml:space="preserve">Ambati Rayudu </v>
+      </c>
+      <c r="B12" t="str">
+        <v>Chennai Super Kings</v>
+      </c>
+      <c r="C12" t="str">
+        <v>42</v>
+      </c>
+      <c r="D12" t="str">
+        <v>40</v>
+      </c>
+      <c r="E12" t="str">
+        <v>4</v>
+      </c>
+      <c r="F12" t="str">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:F11"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:F12"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated till excel part
</commit_message>
<xml_diff>
--- a/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
+++ b/IPL/Chennai Super Kings/Ambati Rayudu .xlsx
@@ -428,16 +428,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C3" t="str">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="D3" t="str">
-        <v>20</v>
+        <v>27</v>
       </c>
       <c r="E3" t="str">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="F3" t="str">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4">
@@ -468,7 +468,7 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C5" t="str">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="D5" t="str">
         <v>27</v>
@@ -477,7 +477,7 @@
         <v>3</v>
       </c>
       <c r="F5" t="str">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6">
@@ -488,13 +488,13 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C6" t="str">
-        <v>30</v>
+        <v>8</v>
       </c>
       <c r="D6" t="str">
-        <v>27</v>
+        <v>9</v>
       </c>
       <c r="E6" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F6" t="str">
         <v>0</v>
@@ -508,16 +508,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C7" t="str">
-        <v>13</v>
+        <v>41</v>
       </c>
       <c r="D7" t="str">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="E7" t="str">
+        <v>3</v>
+      </c>
+      <c r="F7" t="str">
         <v>2</v>
-      </c>
-      <c r="F7" t="str">
-        <v>0</v>
       </c>
     </row>
     <row r="8">
@@ -528,16 +528,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C8" t="str">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D8" t="str">
-        <v>34</v>
+        <v>25</v>
       </c>
       <c r="E8" t="str">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="F8" t="str">
-        <v>2</v>
+        <v>4</v>
       </c>
     </row>
     <row r="9">
@@ -548,16 +548,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C9" t="str">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="D9" t="str">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="E9" t="str">
+        <v>5</v>
+      </c>
+      <c r="F9" t="str">
         <v>1</v>
-      </c>
-      <c r="F9" t="str">
-        <v>4</v>
       </c>
     </row>
     <row r="10">
@@ -568,16 +568,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C10" t="str">
-        <v>8</v>
+        <v>71</v>
       </c>
       <c r="D10" t="str">
-        <v>9</v>
+        <v>48</v>
       </c>
       <c r="E10" t="str">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="F10" t="str">
-        <v>0</v>
+        <v>3</v>
       </c>
     </row>
     <row r="11">
@@ -588,16 +588,16 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C11" t="str">
-        <v>71</v>
+        <v>42</v>
       </c>
       <c r="D11" t="str">
-        <v>48</v>
+        <v>40</v>
       </c>
       <c r="E11" t="str">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="F11" t="str">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="12">
@@ -608,13 +608,13 @@
         <v>Chennai Super Kings</v>
       </c>
       <c r="C12" t="str">
-        <v>42</v>
+        <v>13</v>
       </c>
       <c r="D12" t="str">
-        <v>40</v>
+        <v>19</v>
       </c>
       <c r="E12" t="str">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="F12" t="str">
         <v>0</v>

</xml_diff>